<commit_message>
seguimiento estudio dia 2
noche
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fredo\Documents\GitHub\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F31C320-A1FB-4072-9B02-4822C870198E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41561BD-81D7-4B88-B217-8079380FE9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>Fecha</t>
   </si>
@@ -71,6 +71,10 @@
   <si>
     <t>Mapas en Dart
 Colecciones en Dart</t>
+  </si>
+  <si>
+    <t>Palabras claves cons final dynamic
+Manipulación de String</t>
   </si>
 </sst>
 </file>
@@ -228,23 +232,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,10 +604,10 @@
       <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="9" t="s">
@@ -612,18 +616,18 @@
     </row>
     <row r="6" spans="3:6" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="10"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="10"/>
     </row>
     <row r="7" spans="3:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="9" t="s">
@@ -632,19 +636,29 @@
     </row>
     <row r="8" spans="3:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C8" s="10"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+    <row r="9" spans="3:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="3:6" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C11" s="5"/>
@@ -903,19 +917,72 @@
       <c r="F58" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="91">
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
+  <mergeCells count="92">
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
     <mergeCell ref="F49:F50"/>
@@ -931,70 +998,18 @@
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
     <mergeCell ref="F47:F48"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>